<commit_message>
new results. 2021/03/28 17:15
</commit_message>
<xml_diff>
--- a/res/SEED/result.xlsx
+++ b/res/SEED/result.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hanyiik/Desktop/res/SEED/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hanyiik/PycharmProjects/Finegrained_GNN/res/SEED/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{780D9AFB-3C41-3040-80EA-5BD1814CC942}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01CDE176-807A-224C-B533-DFA1F5F9FE5B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -484,7 +484,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="131" workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
@@ -518,7 +518,7 @@
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="3">
         <v>0.81789999999999996</v>
       </c>
     </row>
@@ -526,7 +526,7 @@
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B5" s="2">
         <v>0.89090000000000003</v>
       </c>
     </row>
@@ -558,7 +558,7 @@
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9" s="4">
+      <c r="B9" s="3">
         <v>0.82440000000000002</v>
       </c>
     </row>
@@ -606,7 +606,7 @@
       <c r="A15">
         <v>14</v>
       </c>
-      <c r="B15" s="4">
+      <c r="B15" s="3">
         <v>0.82730000000000004</v>
       </c>
     </row>
@@ -630,7 +630,7 @@
       <c r="A18">
         <v>17</v>
       </c>
-      <c r="B18" s="4">
+      <c r="B18" s="3">
         <v>0.82010000000000005</v>
       </c>
     </row>
@@ -654,7 +654,7 @@
       <c r="A21">
         <v>20</v>
       </c>
-      <c r="B21" s="4">
+      <c r="B21" s="2">
         <v>0.88290000000000002</v>
       </c>
     </row>
@@ -662,7 +662,7 @@
       <c r="A22">
         <v>21</v>
       </c>
-      <c r="B22" s="4">
+      <c r="B22" s="3">
         <v>0.82230000000000003</v>
       </c>
     </row>
@@ -686,7 +686,7 @@
       <c r="A25">
         <v>24</v>
       </c>
-      <c r="B25" s="4">
+      <c r="B25" s="2">
         <v>0.8952</v>
       </c>
     </row>
@@ -766,7 +766,7 @@
       <c r="A35">
         <v>34</v>
       </c>
-      <c r="B35" s="4">
+      <c r="B35" s="3">
         <v>0.81579999999999997</v>
       </c>
     </row>
@@ -798,7 +798,7 @@
       <c r="A39">
         <v>38</v>
       </c>
-      <c r="B39" s="4">
+      <c r="B39" s="2">
         <v>0.89380000000000004</v>
       </c>
     </row>
@@ -814,7 +814,7 @@
       <c r="A41">
         <v>40</v>
       </c>
-      <c r="B41" s="4">
+      <c r="B41" s="2">
         <v>0.88219999999999998</v>
       </c>
     </row>

</xml_diff>